<commit_message>
ngay 26 thang 8 ver 1
</commit_message>
<xml_diff>
--- a/Bấm giờ Ultra Adventure hat_fix.xlsx
+++ b/Bấm giờ Ultra Adventure hat_fix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\My_PC\OneDrive - VNU-HCMUS\Desktop\SE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F117D73-D31B-4016-A3C6-2F1BF4830223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2C40E6-379C-4D28-A926-9F7C0C954193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Sơ đồ công đoạn 5'!$A$1:$Z$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="81">
   <si>
     <t>Dự bị</t>
   </si>
@@ -301,6 +302,51 @@
   <si>
     <t>BẢNG QUY TRÌNH CÔNG ĐOẠN ULTRA ADVENTURE HAT</t>
   </si>
+  <si>
+    <t>1 người = 0.39</t>
+  </si>
+  <si>
+    <t>1 người = 1.19</t>
+  </si>
+  <si>
+    <t>1 người = 1.27</t>
+  </si>
+  <si>
+    <t>1 người = 0.84</t>
+  </si>
+  <si>
+    <t>1 người = 0.95</t>
+  </si>
+  <si>
+    <t>1 người = 1.26</t>
+  </si>
+  <si>
+    <t>1 người  = 1.38</t>
+  </si>
+  <si>
+    <t>1 người = 1.13</t>
+  </si>
+  <si>
+    <t>1 người = 1.23</t>
+  </si>
+  <si>
+    <t>1 người = 0.77</t>
+  </si>
+  <si>
+    <t>1 người = 0.99</t>
+  </si>
+  <si>
+    <t>1 người = 1.2</t>
+  </si>
+  <si>
+    <t>1 người = 1.3</t>
+  </si>
+  <si>
+    <t>1 người = 1.43</t>
+  </si>
+  <si>
+    <t>1 người = 1.28</t>
+  </si>
 </sst>
 </file>
 
@@ -309,12 +355,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -649,39 +702,39 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -690,64 +743,61 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -759,13 +809,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -777,19 +827,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -798,146 +848,233 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -949,110 +1086,41 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2183,13 +2251,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>11207</xdr:colOff>
+      <xdr:colOff>11206</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>403412</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>470646</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1868</xdr:rowOff>
     </xdr:to>
@@ -2206,8 +2274,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000" flipV="1">
-          <a:off x="8068236" y="1255059"/>
-          <a:ext cx="3664323" cy="360456"/>
+          <a:off x="3966882" y="448236"/>
+          <a:ext cx="2913529" cy="360456"/>
         </a:xfrm>
         <a:prstGeom prst="uturnArrow">
           <a:avLst>
@@ -2508,174 +2576,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>403411</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>33619</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>56029</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>192369</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="101" name="U-Turn Arrow 53">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF5ACA3-2E66-4AA4-808E-CF0CAFB75831}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1" flipV="1">
-          <a:off x="6813176" y="1243854"/>
-          <a:ext cx="2106706" cy="360456"/>
-        </a:xfrm>
-        <a:prstGeom prst="uturnArrow">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 22750"/>
-            <a:gd name="adj2" fmla="val 21925"/>
-            <a:gd name="adj3" fmla="val 17283"/>
-            <a:gd name="adj4" fmla="val 29681"/>
-            <a:gd name="adj5" fmla="val 100000"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="en-US">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-            </a:defRPr>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>616323</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -3016,7 +2916,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="17213950" flipH="1">
-          <a:off x="2270231" y="3896840"/>
+          <a:off x="2270231" y="2877105"/>
           <a:ext cx="158363" cy="2237213"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -3661,7 +3561,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="17986720" flipH="1">
-          <a:off x="3504606" y="4351335"/>
+          <a:off x="3504606" y="3331600"/>
           <a:ext cx="148913" cy="1341592"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
@@ -3987,8 +3887,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="17213950" flipH="1">
-          <a:off x="11338977" y="3817066"/>
-          <a:ext cx="197071" cy="2394475"/>
+          <a:off x="7237624" y="2797331"/>
+          <a:ext cx="197071" cy="2394476"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
           <a:avLst/>
@@ -4787,6 +4687,325 @@
           <a:ext cx="132528" cy="549088"/>
         </a:xfrm>
         <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>616324</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2084294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>789044</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>184785</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Chevron 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1724137B-F2A2-40F9-91E2-44F8396C0A1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14388353" y="3473823"/>
+          <a:ext cx="172720" cy="195991"/>
+        </a:xfrm>
+        <a:prstGeom prst="chevron">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B050"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+            </a:defRPr>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>638736</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2028264</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>201107</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>132117</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Right Arrow 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A20644-6376-4CBA-975B-529606401C11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7866530" y="3417793"/>
+          <a:ext cx="380401" cy="199353"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -10589,13 +10808,15 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="22" width="10.75" style="1" customWidth="1"/>
+    <col min="2" max="15" width="10.75" style="1" customWidth="1"/>
+    <col min="16" max="18" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="10.75" style="1" customWidth="1"/>
     <col min="23" max="27" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -10715,44 +10936,44 @@
     </row>
     <row r="5" spans="1:27">
       <c r="A5" s="14"/>
-      <c r="B5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="93"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="95" t="s">
-        <v>1</v>
+      <c r="B5" s="141" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="140" t="s">
+        <v>67</v>
       </c>
       <c r="F5" s="96"/>
-      <c r="G5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="94"/>
-      <c r="I5" s="95" t="s">
-        <v>1</v>
+      <c r="G5" s="141" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="93"/>
+      <c r="I5" s="140" t="s">
+        <v>75</v>
       </c>
       <c r="J5" s="96"/>
-      <c r="K5" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="94"/>
-      <c r="M5" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="91"/>
-      <c r="O5" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="P5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="R5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="S5" s="18"/>
+      <c r="K5" s="141" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="93"/>
+      <c r="M5" s="143" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="101"/>
+      <c r="O5" s="144" t="s">
+        <v>78</v>
+      </c>
+      <c r="P5" s="145" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q5" s="146" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="146" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="17"/>
       <c r="T5" s="9"/>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
@@ -10770,42 +10991,42 @@
       <c r="C6" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="99" t="s">
+      <c r="D6" s="93"/>
+      <c r="E6" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="97" t="s">
+      <c r="F6" s="95"/>
+      <c r="G6" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="98"/>
-      <c r="I6" s="19" t="s">
+      <c r="H6" s="91"/>
+      <c r="I6" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="98"/>
-      <c r="M6" s="99" t="s">
+      <c r="L6" s="91"/>
+      <c r="M6" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="100"/>
-      <c r="O6" s="21" t="s">
+      <c r="N6" s="95"/>
+      <c r="O6" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="Q6" s="17" t="s">
+      <c r="Q6" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="R6" s="23" t="s">
+      <c r="R6" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="S6" s="18"/>
+      <c r="S6" s="17"/>
       <c r="T6" s="9"/>
       <c r="U6"/>
       <c r="V6"/>
@@ -10816,226 +11037,226 @@
       <c r="AA6"/>
     </row>
     <row r="7" spans="1:27" s="2" customFormat="1" ht="165">
-      <c r="A7" s="24"/>
-      <c r="B7" s="21" t="s">
+      <c r="A7" s="23"/>
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="98"/>
-      <c r="M7" s="23" t="s">
+      <c r="L7" s="91"/>
+      <c r="M7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="21" t="s">
+      <c r="O7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q7" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="S7" s="26"/>
+      <c r="S7" s="25"/>
       <c r="T7" s="7"/>
     </row>
     <row r="8" spans="1:27" s="2" customFormat="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="21">
+      <c r="A8" s="25"/>
+      <c r="B8" s="20">
         <v>16</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>12</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>13</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="22">
         <v>22</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>23</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>24</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="20">
         <v>25</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
+        <v>11</v>
+      </c>
+      <c r="J8" s="22">
         <v>6</v>
       </c>
-      <c r="J8" s="23">
-        <v>11</v>
-      </c>
-      <c r="K8" s="97">
+      <c r="K8" s="90">
         <v>7</v>
       </c>
-      <c r="L8" s="98"/>
-      <c r="M8" s="23">
+      <c r="L8" s="91"/>
+      <c r="M8" s="22">
         <v>31</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="22">
         <v>32</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="20">
         <v>28</v>
       </c>
-      <c r="P8" s="22">
+      <c r="P8" s="21">
         <v>30</v>
       </c>
-      <c r="Q8" s="23">
+      <c r="Q8" s="22">
         <v>33</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="22">
         <v>34</v>
       </c>
-      <c r="S8" s="26"/>
+      <c r="S8" s="25"/>
       <c r="T8" s="7"/>
     </row>
     <row r="9" spans="1:27" s="3" customFormat="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="101"/>
-      <c r="R9" s="101"/>
-      <c r="S9" s="27"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="97"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="26"/>
     </row>
     <row r="10" spans="1:27" s="3" customFormat="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="101"/>
-      <c r="Q10" s="101"/>
-      <c r="R10" s="101"/>
-      <c r="S10" s="26"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="97"/>
+      <c r="I10" s="97"/>
+      <c r="J10" s="97"/>
+      <c r="K10" s="97"/>
+      <c r="L10" s="97"/>
+      <c r="M10" s="97"/>
+      <c r="N10" s="97"/>
+      <c r="O10" s="97"/>
+      <c r="P10" s="97"/>
+      <c r="Q10" s="97"/>
+      <c r="R10" s="97"/>
+      <c r="S10" s="25"/>
     </row>
     <row r="11" spans="1:27" s="3" customFormat="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
-      <c r="L11" s="101"/>
-      <c r="M11" s="101"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="101"/>
-      <c r="P11" s="101"/>
-      <c r="Q11" s="101"/>
-      <c r="R11" s="101"/>
-      <c r="S11" s="26"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="97"/>
+      <c r="Q11" s="97"/>
+      <c r="R11" s="97"/>
+      <c r="S11" s="25"/>
     </row>
     <row r="12" spans="1:27" s="2" customFormat="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="21">
+      <c r="A12" s="25"/>
+      <c r="B12" s="20">
         <v>15</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>14</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>10</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>17</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>18</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <v>19</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <v>21</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="16">
         <v>20</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="16">
         <v>4</v>
       </c>
-      <c r="K12" s="97">
+      <c r="K12" s="90">
         <v>26</v>
       </c>
-      <c r="L12" s="98"/>
-      <c r="M12" s="99">
+      <c r="L12" s="91"/>
+      <c r="M12" s="94">
         <v>5</v>
       </c>
-      <c r="N12" s="100"/>
-      <c r="O12" s="21">
+      <c r="N12" s="95"/>
+      <c r="O12" s="20">
         <v>27</v>
       </c>
-      <c r="P12" s="21">
+      <c r="P12" s="20">
         <v>29</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="Q12" s="22">
         <v>8</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="22">
         <v>9</v>
       </c>
-      <c r="S12" s="26"/>
+      <c r="S12" s="25"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
       <c r="V12" s="7"/>
@@ -11045,55 +11266,55 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:27" s="2" customFormat="1" ht="146.25" customHeight="1">
-      <c r="A13" s="24"/>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="97" t="s">
+      <c r="K13" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99" t="s">
+      <c r="L13" s="91"/>
+      <c r="M13" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="N13" s="100"/>
-      <c r="O13" s="21" t="s">
+      <c r="N13" s="95"/>
+      <c r="O13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="23" t="s">
+      <c r="Q13" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="R13" s="23" t="s">
+      <c r="R13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="S13" s="26"/>
+      <c r="S13" s="25"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
@@ -11103,43 +11324,43 @@
       <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:27" s="3" customFormat="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="97" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="103"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="99" t="s">
+      <c r="C14" s="100"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="100"/>
-      <c r="G14" s="97" t="s">
+      <c r="F14" s="95"/>
+      <c r="G14" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="98"/>
-      <c r="I14" s="30" t="s">
+      <c r="H14" s="91"/>
+      <c r="I14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="K14" s="97" t="s">
+      <c r="K14" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="98"/>
-      <c r="M14" s="99" t="s">
+      <c r="L14" s="91"/>
+      <c r="M14" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="100"/>
-      <c r="O14" s="101" t="s">
+      <c r="N14" s="95"/>
+      <c r="O14" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="P14" s="101"/>
-      <c r="Q14" s="99" t="s">
+      <c r="P14" s="97"/>
+      <c r="Q14" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="100"/>
-      <c r="S14" s="26"/>
+      <c r="R14" s="95"/>
+      <c r="S14" s="25"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
@@ -11150,37 +11371,37 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" s="14"/>
-      <c r="B15" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="95" t="s">
-        <v>1</v>
+      <c r="B15" s="141" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="99"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="140" t="s">
+        <v>70</v>
       </c>
       <c r="F15" s="96"/>
-      <c r="G15" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="94"/>
-      <c r="I15" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="102"/>
-      <c r="K15" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="94"/>
-      <c r="M15" s="95" t="s">
-        <v>49</v>
+      <c r="G15" s="141" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="93"/>
+      <c r="I15" s="140" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="98"/>
+      <c r="K15" s="141" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" s="93"/>
+      <c r="M15" s="140" t="s">
+        <v>72</v>
       </c>
       <c r="N15" s="96"/>
-      <c r="O15" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="P15" s="94"/>
-      <c r="Q15" s="95" t="s">
-        <v>1</v>
+      <c r="O15" s="141" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="140" t="s">
+        <v>74</v>
       </c>
       <c r="R15" s="96"/>
       <c r="S15" s="14"/>
@@ -11633,12 +11854,17 @@
     <row r="35" customFormat="1"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="B9:R11"/>
     <mergeCell ref="Q14:R14"/>
@@ -11655,17 +11881,12 @@
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M13:N13"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.1" right="0.1" top="0.1" bottom="0.1" header="0.1" footer="0.1"/>
@@ -11682,7 +11903,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -11769,502 +11990,502 @@
       <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25">
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="139"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="138" t="s">
+      <c r="C4" s="103"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="139"/>
-      <c r="G4" s="140"/>
-      <c r="H4" s="110" t="s">
+      <c r="F4" s="103"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="112"/>
-      <c r="J4" s="113" t="s">
+      <c r="I4" s="106"/>
+      <c r="J4" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="114"/>
-      <c r="L4" s="110" t="s">
+      <c r="K4" s="108"/>
+      <c r="L4" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="112"/>
-      <c r="N4" s="113" t="s">
+      <c r="M4" s="106"/>
+      <c r="N4" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="114"/>
-      <c r="P4" s="31" t="s">
+      <c r="O4" s="108"/>
+      <c r="P4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="32" t="s">
+      <c r="Q4" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="113" t="s">
+      <c r="R4" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="114"/>
-      <c r="T4" s="31" t="s">
+      <c r="S4" s="108"/>
+      <c r="T4" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="U4" s="33" t="s">
+      <c r="U4" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="31.5">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="49" t="s">
+      <c r="C5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="133" t="s">
+      <c r="E5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="134"/>
-      <c r="G5" s="34" t="s">
+      <c r="F5" s="116"/>
+      <c r="G5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="121" t="s">
+      <c r="H5" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="122"/>
-      <c r="J5" s="133" t="s">
+      <c r="I5" s="118"/>
+      <c r="J5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="134"/>
-      <c r="L5" s="35" t="s">
+      <c r="K5" s="116"/>
+      <c r="L5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="34" t="s">
+      <c r="O5" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="31" t="s">
+      <c r="P5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="36" t="s">
+      <c r="Q5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="R5" s="133" t="s">
+      <c r="R5" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="134"/>
-      <c r="T5" s="35" t="s">
+      <c r="S5" s="116"/>
+      <c r="T5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="34" t="s">
+      <c r="U5" s="33" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="140.25">
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C6" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D6" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="38" t="s">
+      <c r="I6" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="37" t="s">
+      <c r="K6" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="38" t="s">
+      <c r="L6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="39" t="s">
+      <c r="Q6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="37" t="s">
+      <c r="R6" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="S6" s="37" t="s">
+      <c r="S6" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="T6" s="38" t="s">
+      <c r="T6" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="U6" s="37" t="s">
+      <c r="U6" s="36" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:25">
-      <c r="B7" s="50">
+      <c r="B7" s="49">
         <v>18</v>
       </c>
-      <c r="C7" s="50">
+      <c r="C7" s="49">
         <v>17</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="49">
         <v>8</v>
       </c>
-      <c r="E7" s="135">
+      <c r="E7" s="119">
         <v>9</v>
       </c>
-      <c r="F7" s="136"/>
-      <c r="G7" s="37">
+      <c r="F7" s="120"/>
+      <c r="G7" s="36">
         <v>10</v>
       </c>
-      <c r="H7" s="137">
+      <c r="H7" s="121">
         <v>11</v>
       </c>
-      <c r="I7" s="137"/>
-      <c r="J7" s="135">
+      <c r="I7" s="121"/>
+      <c r="J7" s="119">
         <v>12</v>
       </c>
-      <c r="K7" s="136"/>
-      <c r="L7" s="38">
+      <c r="K7" s="120"/>
+      <c r="L7" s="37">
         <v>3</v>
       </c>
-      <c r="M7" s="38">
+      <c r="M7" s="37">
         <v>21</v>
       </c>
-      <c r="N7" s="37">
+      <c r="N7" s="36">
         <v>5</v>
       </c>
-      <c r="O7" s="37">
+      <c r="O7" s="36">
         <v>22</v>
       </c>
-      <c r="P7" s="39">
+      <c r="P7" s="38">
         <v>23</v>
       </c>
-      <c r="Q7" s="39">
+      <c r="Q7" s="38">
         <v>24</v>
       </c>
-      <c r="R7" s="37">
+      <c r="R7" s="36">
         <v>29</v>
       </c>
-      <c r="S7" s="37">
+      <c r="S7" s="36">
         <v>30</v>
       </c>
-      <c r="T7" s="39">
+      <c r="T7" s="38">
         <v>31</v>
       </c>
-      <c r="U7" s="37">
+      <c r="U7" s="36">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:25">
       <c r="A8" s="3"/>
-      <c r="B8" s="123"/>
-      <c r="C8" s="124"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="123"/>
-      <c r="O8" s="125"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="123"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="123"/>
-      <c r="U8" s="125"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="110"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="125"/>
+      <c r="J8" s="125"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="109"/>
+      <c r="O8" s="110"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="110"/>
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="3"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="125"/>
+      <c r="I9" s="125"/>
+      <c r="J9" s="125"/>
       <c r="K9" s="10"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="126"/>
-      <c r="O9" s="128"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="126"/>
-      <c r="S9" s="128"/>
-      <c r="T9" s="126"/>
-      <c r="U9" s="128"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="111"/>
+      <c r="O9" s="112"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="111"/>
+      <c r="S9" s="112"/>
+      <c r="T9" s="111"/>
+      <c r="U9" s="112"/>
     </row>
     <row r="10" spans="1:25">
       <c r="A10" s="3"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="130"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="129"/>
-      <c r="O10" s="131"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="129"/>
-      <c r="S10" s="131"/>
-      <c r="T10" s="129"/>
-      <c r="U10" s="131"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="125"/>
+      <c r="I10" s="125"/>
+      <c r="J10" s="125"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="113"/>
+      <c r="O10" s="114"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="113"/>
+      <c r="S10" s="114"/>
+      <c r="T10" s="113"/>
+      <c r="U10" s="114"/>
     </row>
     <row r="11" spans="1:25">
-      <c r="B11" s="37"/>
-      <c r="C11" s="115">
+      <c r="B11" s="36"/>
+      <c r="C11" s="126">
         <v>13</v>
       </c>
-      <c r="D11" s="116"/>
-      <c r="E11" s="50">
+      <c r="D11" s="127"/>
+      <c r="E11" s="49">
         <v>15</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <v>14</v>
       </c>
-      <c r="G11" s="37">
+      <c r="G11" s="36">
         <v>16</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="42">
         <v>19</v>
       </c>
-      <c r="I11" s="38">
+      <c r="I11" s="37">
         <v>1</v>
       </c>
-      <c r="J11" s="117">
+      <c r="J11" s="128">
         <v>2</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="37">
+      <c r="K11" s="129"/>
+      <c r="L11" s="36">
         <v>4</v>
       </c>
-      <c r="M11" s="37">
+      <c r="M11" s="36">
         <v>20</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="43">
         <v>6</v>
       </c>
-      <c r="O11" s="44">
+      <c r="O11" s="43">
         <v>7</v>
       </c>
-      <c r="P11" s="37">
+      <c r="P11" s="36">
         <v>25</v>
       </c>
-      <c r="Q11" s="37">
+      <c r="Q11" s="36">
         <v>26</v>
       </c>
-      <c r="R11" s="38">
+      <c r="R11" s="37">
         <v>27</v>
       </c>
-      <c r="S11" s="37">
+      <c r="S11" s="36">
         <v>28</v>
       </c>
-      <c r="T11" s="38">
+      <c r="T11" s="37">
         <v>28</v>
       </c>
-      <c r="U11" s="37">
+      <c r="U11" s="36">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="140.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="K12" s="38" t="s">
+      <c r="K12" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="L12" s="45" t="s">
+      <c r="L12" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="M12" s="45" t="s">
+      <c r="M12" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="38" t="s">
+      <c r="N12" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="38" t="s">
+      <c r="O12" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="P12" s="37" t="s">
+      <c r="P12" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="Q12" s="37" t="s">
+      <c r="Q12" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="38" t="s">
+      <c r="R12" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="S12" s="37" t="s">
+      <c r="S12" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="T12" s="38" t="s">
+      <c r="T12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="U12" s="37" t="s">
+      <c r="U12" s="36" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="31.5">
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="119" t="s">
+      <c r="C13" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="120"/>
-      <c r="E13" s="48" t="s">
+      <c r="D13" s="131"/>
+      <c r="E13" s="47" t="s">
         <v>3</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="47" t="s">
+      <c r="I13" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="121" t="s">
+      <c r="J13" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="K13" s="122"/>
-      <c r="L13" s="34" t="s">
+      <c r="K13" s="118"/>
+      <c r="L13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="N13" s="121" t="s">
+      <c r="N13" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="O13" s="122"/>
-      <c r="P13" s="34" t="s">
+      <c r="O13" s="118"/>
+      <c r="P13" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="Q13" s="34" t="s">
+      <c r="Q13" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="R13" s="47" t="s">
+      <c r="R13" s="46" t="s">
         <v>6</v>
       </c>
       <c r="S13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="T13" s="47" t="s">
+      <c r="T13" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="U13" s="34" t="s">
+      <c r="U13" s="33" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="107" t="s">
+      <c r="D14" s="133"/>
+      <c r="E14" s="134"/>
+      <c r="F14" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="G14" s="108"/>
-      <c r="H14" s="109"/>
-      <c r="I14" s="110" t="s">
+      <c r="G14" s="136"/>
+      <c r="H14" s="137"/>
+      <c r="I14" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="J14" s="111"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="113" t="s">
+      <c r="J14" s="138"/>
+      <c r="K14" s="106"/>
+      <c r="L14" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="M14" s="114"/>
-      <c r="N14" s="110" t="s">
+      <c r="M14" s="108"/>
+      <c r="N14" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="112"/>
-      <c r="P14" s="113" t="s">
+      <c r="O14" s="106"/>
+      <c r="P14" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="Q14" s="114"/>
-      <c r="R14" s="31" t="s">
+      <c r="Q14" s="108"/>
+      <c r="R14" s="30" t="s">
         <v>1</v>
       </c>
       <c r="S14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="T14" s="31" t="s">
+      <c r="T14" s="30" t="s">
         <v>1</v>
       </c>
       <c r="U14" s="12" t="s">
@@ -12356,26 +12577,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="T8:U10"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B8:D10"/>
-    <mergeCell ref="E8:G10"/>
-    <mergeCell ref="H8:J10"/>
-    <mergeCell ref="N8:O10"/>
-    <mergeCell ref="R8:S10"/>
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="J11:K11"/>
@@ -12387,6 +12588,26 @@
     <mergeCell ref="I14:K14"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="N14:O14"/>
+    <mergeCell ref="B8:D10"/>
+    <mergeCell ref="E8:G10"/>
+    <mergeCell ref="H8:J10"/>
+    <mergeCell ref="N8:O10"/>
+    <mergeCell ref="R8:S10"/>
+    <mergeCell ref="T8:U10"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12398,787 +12619,787 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="4.25" style="53" customWidth="1"/>
-    <col min="2" max="2" width="42.125" style="51" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="81" customWidth="1"/>
-    <col min="4" max="5" width="10.75" style="53" customWidth="1"/>
-    <col min="6" max="6" width="14.625" style="51" customWidth="1"/>
-    <col min="7" max="9" width="14.625" style="52" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="51"/>
+    <col min="1" max="1" width="4.25" style="52" customWidth="1"/>
+    <col min="2" max="2" width="42.125" style="50" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="80" customWidth="1"/>
+    <col min="4" max="5" width="10.75" style="52" customWidth="1"/>
+    <col min="6" max="6" width="14.625" style="50" customWidth="1"/>
+    <col min="7" max="9" width="14.625" style="51" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="50"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="79" customFormat="1" ht="27" customHeight="1">
-      <c r="A1" s="141" t="s">
+    <row r="1" spans="1:9" s="78" customFormat="1" ht="27" customHeight="1">
+      <c r="A1" s="139" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
+      <c r="B1" s="139"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="139"/>
+      <c r="E1" s="139"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
     </row>
     <row r="2" spans="1:9" ht="33.950000000000003" customHeight="1">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="77" t="s">
+      <c r="D2" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="77" t="s">
+      <c r="G2" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="H2" s="77" t="s">
+      <c r="H2" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="76" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A3" s="82">
+      <c r="A3" s="81">
         <v>1</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="84">
         <v>1</v>
       </c>
-      <c r="E3" s="86"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
     </row>
     <row r="4" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A4" s="82">
+      <c r="A4" s="81">
         <v>2</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="85">
+      <c r="D4" s="84">
         <v>1</v>
       </c>
-      <c r="E4" s="88"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
     </row>
     <row r="5" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A5" s="82">
+      <c r="A5" s="81">
         <v>3</v>
       </c>
-      <c r="B5" s="83" t="s">
+      <c r="B5" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="84">
         <v>1</v>
       </c>
-      <c r="E5" s="88"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
     </row>
     <row r="6" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A6" s="60">
+      <c r="A6" s="59">
         <v>4</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="60">
         <v>1</v>
       </c>
-      <c r="E6" s="58"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A7" s="60">
+      <c r="A7" s="59">
         <v>5</v>
       </c>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="60">
         <v>1</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
     </row>
     <row r="8" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A8" s="60">
+      <c r="A8" s="59">
         <v>6</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="61">
+      <c r="D8" s="60">
         <v>1</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
     </row>
     <row r="9" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A9" s="60">
+      <c r="A9" s="59">
         <v>7</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="61">
+      <c r="D9" s="60">
         <v>1</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="56"/>
     </row>
     <row r="10" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A10" s="60">
+      <c r="A10" s="59">
         <v>8</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="60">
         <v>1</v>
       </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
     </row>
     <row r="11" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A11" s="60">
+      <c r="A11" s="59">
         <v>9</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="61">
+      <c r="D11" s="60">
         <v>1</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A12" s="60">
+      <c r="A12" s="59">
         <v>10</v>
       </c>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="61">
+      <c r="D12" s="60">
         <v>1</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
     </row>
     <row r="13" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A13" s="60">
+      <c r="A13" s="59">
         <v>11</v>
       </c>
-      <c r="B13" s="62" t="s">
+      <c r="B13" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="60">
         <v>1</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A14" s="76">
+      <c r="A14" s="75">
         <v>12</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="71" t="s">
+      <c r="C14" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="70">
+      <c r="D14" s="69">
         <v>1</v>
       </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="75"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
     </row>
     <row r="15" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A15" s="73">
+      <c r="A15" s="72">
         <v>13</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="71" t="s">
+      <c r="C15" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="70">
+      <c r="D15" s="69">
         <v>1</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="57"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A16" s="60">
+      <c r="A16" s="59">
         <v>14</v>
       </c>
-      <c r="B16" s="62" t="s">
+      <c r="B16" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="61">
+      <c r="D16" s="60">
         <v>1</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A17" s="60">
+      <c r="A17" s="59">
         <v>15</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="61">
+      <c r="D17" s="60">
         <v>1</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A18" s="73">
+      <c r="A18" s="72">
         <v>16</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="70">
+      <c r="D18" s="69">
         <v>1</v>
       </c>
-      <c r="E18" s="69"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A19" s="60">
+      <c r="A19" s="59">
         <v>17</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="61">
+      <c r="D19" s="60">
         <v>1</v>
       </c>
-      <c r="E19" s="58"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
     </row>
     <row r="20" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A20" s="60">
+      <c r="A20" s="59">
         <v>18</v>
       </c>
-      <c r="B20" s="62" t="s">
+      <c r="B20" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="61">
+      <c r="D20" s="60">
         <v>1</v>
       </c>
-      <c r="E20" s="58"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
     </row>
     <row r="21" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A21" s="60">
+      <c r="A21" s="59">
         <v>19</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="B21" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="61">
+      <c r="D21" s="60">
         <v>1</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
     </row>
     <row r="22" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A22" s="60">
+      <c r="A22" s="59">
         <v>20</v>
       </c>
-      <c r="B22" s="62" t="s">
+      <c r="B22" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="61">
+      <c r="D22" s="60">
         <v>1</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="57"/>
-      <c r="I22" s="57"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A23" s="60">
+      <c r="A23" s="59">
         <v>21</v>
       </c>
-      <c r="B23" s="62" t="s">
+      <c r="B23" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="61">
+      <c r="D23" s="60">
         <v>1</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="57"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
     </row>
     <row r="24" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A24" s="60">
+      <c r="A24" s="59">
         <v>22</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="61">
+      <c r="D24" s="60">
         <v>1</v>
       </c>
-      <c r="E24" s="58"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="57"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
     </row>
     <row r="25" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A25" s="60">
+      <c r="A25" s="59">
         <v>23</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="61">
+      <c r="D25" s="60">
         <v>1</v>
       </c>
-      <c r="E25" s="58"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
     </row>
     <row r="26" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A26" s="60">
+      <c r="A26" s="59">
         <v>24</v>
       </c>
-      <c r="B26" s="62" t="s">
+      <c r="B26" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="66" t="s">
+      <c r="C26" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="61">
+      <c r="D26" s="60">
         <v>1</v>
       </c>
-      <c r="E26" s="58"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
     </row>
     <row r="27" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A27" s="60">
+      <c r="A27" s="59">
         <v>25</v>
       </c>
-      <c r="B27" s="62" t="s">
+      <c r="B27" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="66" t="s">
+      <c r="C27" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="60">
         <v>1</v>
       </c>
-      <c r="E27" s="58"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="68"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
     </row>
     <row r="28" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A28" s="60">
+      <c r="A28" s="59">
         <v>26</v>
       </c>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="61">
+      <c r="D28" s="60">
         <v>1</v>
       </c>
-      <c r="E28" s="63"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
     </row>
     <row r="29" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A29" s="60">
+      <c r="A29" s="59">
         <v>27</v>
       </c>
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="66" t="s">
+      <c r="C29" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="61">
+      <c r="D29" s="60">
         <v>1</v>
       </c>
-      <c r="E29" s="63"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
     </row>
     <row r="30" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A30" s="60">
+      <c r="A30" s="59">
         <v>28</v>
       </c>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C30" s="66" t="s">
+      <c r="C30" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="61">
+      <c r="D30" s="60">
         <v>1</v>
       </c>
-      <c r="E30" s="63"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
     </row>
     <row r="31" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A31" s="60">
+      <c r="A31" s="59">
         <v>29</v>
       </c>
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="66" t="s">
+      <c r="C31" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="61">
+      <c r="D31" s="60">
         <v>1</v>
       </c>
-      <c r="E31" s="58"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
     </row>
     <row r="32" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A32" s="60">
+      <c r="A32" s="59">
         <v>30</v>
       </c>
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="C32" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="61">
+      <c r="D32" s="60">
         <v>1</v>
       </c>
-      <c r="E32" s="58"/>
-      <c r="F32" s="57"/>
-      <c r="G32" s="57"/>
-      <c r="H32" s="57"/>
-      <c r="I32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
     </row>
     <row r="33" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A33" s="60">
+      <c r="A33" s="59">
         <v>31</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="66" t="s">
+      <c r="C33" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="61">
+      <c r="D33" s="60">
         <v>1</v>
       </c>
-      <c r="E33" s="58"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
+      <c r="E33" s="57"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
     </row>
     <row r="34" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A34" s="60">
+      <c r="A34" s="59">
         <v>32</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="B34" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="66" t="s">
+      <c r="C34" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="61">
+      <c r="D34" s="60">
         <v>1</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="56"/>
+      <c r="G34" s="56"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
     </row>
     <row r="35" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A35" s="60">
+      <c r="A35" s="59">
         <v>33</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="66" t="s">
+      <c r="C35" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="61">
+      <c r="D35" s="60">
         <v>1</v>
       </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="57"/>
-      <c r="G35" s="57"/>
-      <c r="H35" s="57"/>
-      <c r="I35" s="57"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
     </row>
     <row r="36" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A36" s="60">
+      <c r="A36" s="59">
         <v>34</v>
       </c>
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="61">
+      <c r="D36" s="60">
         <v>1</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="57"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="57"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="56"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A37" s="82">
+      <c r="A37" s="81">
         <v>35</v>
       </c>
-      <c r="B37" s="83" t="s">
+      <c r="B37" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="84" t="s">
+      <c r="C37" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="85">
+      <c r="D37" s="84">
         <v>1</v>
       </c>
-      <c r="E37" s="88"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
-      <c r="I37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="86"/>
+      <c r="I37" s="86"/>
     </row>
     <row r="38" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A38" s="82">
+      <c r="A38" s="81">
         <v>36</v>
       </c>
-      <c r="B38" s="89" t="s">
+      <c r="B38" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="84" t="s">
+      <c r="C38" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="85">
+      <c r="D38" s="84">
         <v>1</v>
       </c>
-      <c r="E38" s="88"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="87"/>
-      <c r="I38" s="87"/>
+      <c r="E38" s="87"/>
+      <c r="F38" s="86"/>
+      <c r="G38" s="86"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
     </row>
     <row r="39" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A39" s="82">
+      <c r="A39" s="81">
         <v>37</v>
       </c>
-      <c r="B39" s="89" t="s">
+      <c r="B39" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="84" t="s">
+      <c r="C39" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D39" s="90">
+      <c r="D39" s="89">
         <v>1</v>
       </c>
-      <c r="E39" s="88"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="87"/>
-      <c r="I39" s="87"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="86"/>
     </row>
     <row r="40" spans="1:9" ht="26.1" customHeight="1">
-      <c r="A40" s="82">
+      <c r="A40" s="81">
         <v>38</v>
       </c>
-      <c r="B40" s="89" t="s">
+      <c r="B40" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="84" t="s">
+      <c r="C40" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="90">
+      <c r="D40" s="89">
         <v>1</v>
       </c>
-      <c r="E40" s="88"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="87"/>
-      <c r="I40" s="87"/>
+      <c r="E40" s="87"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
     </row>
     <row r="41" spans="1:9" ht="21">
-      <c r="D41" s="56"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="54"/>
+      <c r="D41" s="55"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>